<commit_message>
Add Normal sheet in excel file and change the way combobox buzaicd display
</commit_message>
<xml_diff>
--- a/Arent3d.Architecture.Routing.AppBase/resources/ElectricalCategory.xlsx
+++ b/Arent3d.Architecture.Routing.AppBase/resources/ElectricalCategory.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Eco" sheetId="1" r:id="rId1"/>
+    <sheet name="Normal" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
   <si>
     <t>【電線】</t>
   </si>
@@ -509,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -676,4 +677,167 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75">
+      <c r="A9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.75">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" ht="15.75">
+      <c r="A16" s="2"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" ht="15.75">
+      <c r="A17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>